<commit_message>
Fixed server.py for Render
</commit_message>
<xml_diff>
--- a/parsed_excels/News_data_Interfax_Today_Yesterday.xlsx
+++ b/parsed_excels/News_data_Interfax_Today_Yesterday.xlsx
@@ -439,7 +439,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C56"/>
+  <dimension ref="A1:C105"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -447,7 +447,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="101" customWidth="1" min="1" max="1"/>
+    <col width="115" customWidth="1" min="1" max="1"/>
     <col width="42" customWidth="1" min="2" max="2"/>
     <col width="18" customWidth="1" min="3" max="3"/>
   </cols>
@@ -472,935 +472,1768 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Поставки ПК в мире во II квартале выросли на 6,5%</t>
+          <t>Brookfield купит 19,7% "дочки" Duke Energy за $6 млрд</t>
         </is>
       </c>
       <c r="B2" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039310</t>
+          <t>https://www.interfax.ru/business/1039790</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01-08-2025 20:40</t>
+          <t>05-08-2025 19:34</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Гонконгская фондовая биржа смягчит некоторые правила листинга</t>
+          <t>Эксперты отметили уязвимость более 60% компаний РФ перед кибервзломом за одни сутки</t>
         </is>
       </c>
       <c r="B3" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039309</t>
+          <t>https://www.interfax.ru/business/1039787</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01-08-2025 20:10</t>
+          <t>05-08-2025 19:32</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Чистая прибыль АЛРОСА в I полугодии выросла на 12% при падении выручки</t>
+          <t>Рубль снизился во вторник вслед за нефтью и в ожидании важных геополитических новостей</t>
         </is>
       </c>
       <c r="B4" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039306</t>
+          <t>https://www.interfax.ru/business/1039788</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>01-08-2025 19:49</t>
+          <t>05-08-2025 19:24</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Uniper закупит газ в Канаде для доставки на биржу в США, откуда компания получит СПГ</t>
+          <t>Рынок акций РФ во вторник продолжил подъем в ожидании геополитических новостей</t>
         </is>
       </c>
       <c r="B5" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039304</t>
+          <t>https://www.interfax.ru/business/1039786</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>01-08-2025 19:39</t>
+          <t>05-08-2025 18:57</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Российский рынок акций завершил пятницу и неделю снижением из-за рисков санкций США</t>
+          <t>Бриллианты в июле продолжили дешеветь на опасениях о пошлинах США</t>
         </is>
       </c>
       <c r="B6" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039296</t>
+          <t>https://www.interfax.ru/business/1039783</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>01-08-2025 19:01</t>
+          <t>05-08-2025 18:49</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Во Франции госсубсидии на ВИЭ в 2026 году вырастут на 23% - до рекордных 9 млрд евро</t>
+          <t>ЕК одобрила программу на 11 млрд евро для внедрения ветроэнергетики во Франции</t>
         </is>
       </c>
       <c r="B7" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/world/1039294</t>
+          <t>https://www.interfax.ru/business/1039782</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>01-08-2025 18:57</t>
+          <t>05-08-2025 18:46</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Цена нефти Brent опустилась до $69,84 за баррель</t>
+          <t>Marathon Petroleum сократила квартальную чистую прибыль на 20%</t>
         </is>
       </c>
       <c r="B8" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039289</t>
+          <t>https://www.interfax.ru/business/1039780</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>01-08-2025 18:34</t>
+          <t>05-08-2025 18:27</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>ЮГК во I полугодии снизила выручку по РСБУ на 22%</t>
+          <t>Brent остается в минусе и торгуется у $68 за баррель</t>
         </is>
       </c>
       <c r="B9" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039290</t>
+          <t>https://www.interfax.ru/business/1039774</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>01-08-2025 18:33</t>
+          <t>05-08-2025 18:01</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Gartner спрогнозировал рост мировых IT-расходов в 2025 году на 7,9%</t>
+          <t>В ЕК не видят в соглашении с США помеху диверсификации энергоисточников</t>
         </is>
       </c>
       <c r="B10" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/digital/1039288</t>
+          <t>https://www.interfax.ru/business/1039772</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>01-08-2025 18:14</t>
+          <t>05-08-2025 17:42</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>Минтранс сохраняет прогноз перевозок российских авиакомпаний на уровне прошлого года</t>
+          <t>Количество выявленных ЦБ "нелегалов" на финрынке в I полугодии выросло на 20%</t>
         </is>
       </c>
       <c r="B11" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/russia/1039287</t>
+          <t>https://www.interfax.ru/business/1039770</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>01-08-2025 18:07</t>
+          <t>05-08-2025 17:37</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Объем торгов "Мосбиржи" в июле вырос на 16% г/г, до 149 трлн рублей</t>
+          <t>"Ростелеком" ждет по итогам 2025 года положительный FCF в размере около 20 млрд рублей</t>
         </is>
       </c>
       <c r="B12" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039283</t>
+          <t>https://www.interfax.ru/business/1039771</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>01-08-2025 17:37</t>
+          <t>05-08-2025 17:35</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>В США в июле индекс потребдоверия вырос слабее прогноза</t>
+          <t>ВР отмечает низкие коммерческие запасы нефти на рынке</t>
         </is>
       </c>
       <c r="B13" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039282</t>
+          <t>https://www.interfax.ru/business/1039769</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>01-08-2025 17:35</t>
+          <t>05-08-2025 17:32</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>В США индекс ISM Manufacturing в июле неожиданно снизился до 48 пунктов</t>
+          <t>Индекс активности в сфере услуг США в июле неожиданно снизился до 50,1 пункта</t>
         </is>
       </c>
       <c r="B14" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039279</t>
+          <t>https://www.interfax.ru/world/1039765</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>01-08-2025 17:17</t>
+          <t>05-08-2025 17:08</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>"ПроЗерно" повысило прогноз сбора урожая в России в 2025 году до 131,3 млн тонн</t>
+          <t>Marriott во II квартале увеличила выручку лучше ожиданий</t>
         </is>
       </c>
       <c r="B15" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039277</t>
+          <t>https://www.interfax.ru/business/1039764</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>01-08-2025 17:07</t>
+          <t>05-08-2025 17:07</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>ЦБ разрешил покупать валюту инвесторам из недружественных стран для новых инвестиций со счетов "Ин"</t>
+          <t>Решение о возможности дивидендов "Норникеля" примут по итогам года с учетом FCF и уровня долга</t>
         </is>
       </c>
       <c r="B16" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039275</t>
+          <t>https://www.interfax.ru/business/1039763</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>01-08-2025 17:02</t>
+          <t>05-08-2025 16:58</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>"Молдовагаз" будет лишен лицензии на поставку газа в Молдавию 4 августа</t>
+          <t>"Норникель" ждет снижения оборотного капитала к концу 2025 года до менее $3 млрд</t>
         </is>
       </c>
       <c r="B17" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/world/1039273</t>
+          <t>https://www.interfax.ru/business/1039762</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>01-08-2025 16:55</t>
+          <t>05-08-2025 16:55</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>XPeng и Xiaomi в июле увеличили поставки электромобилей до рекордных объемов</t>
+          <t>Saudi Aramco ожидает во II полугодии роста спроса на нефть на 2 млн б/с</t>
         </is>
       </c>
       <c r="B18" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039271</t>
+          <t>https://www.interfax.ru/business/1039760</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>01-08-2025 16:54</t>
+          <t>05-08-2025 16:50</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>"КАМАЗ" в I полугодии получил 20,8 млрд руб. чистого убытка по РСБУ</t>
+          <t>Новая стратегия "Ростелекома" может быть осенью представлена совету директоров</t>
         </is>
       </c>
       <c r="B19" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039272</t>
+          <t>https://www.interfax.ru/business/1039758</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>01-08-2025 16:53</t>
+          <t>05-08-2025 16:43</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Предприниматель из Грозного приобрел "субсидиарку" Ванеева по долгам "Евродона"</t>
+          <t>"Ашан" в России сменит гендиректора</t>
         </is>
       </c>
       <c r="B20" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039270</t>
+          <t>https://www.interfax.ru/business/1039752</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>01-08-2025 16:47</t>
+          <t>05-08-2025 16:07</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>"Транснефть" увеличила полугодовую чистую прибыль по РСБУ до 76,3 млрд рублей</t>
+          <t>Минфин 6 августа проведет аукционы по размещению ОФЗ 26248 и 26225</t>
         </is>
       </c>
       <c r="B21" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039266</t>
+          <t>https://www.interfax.ru/russia/1039750</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>01-08-2025 16:25</t>
+          <t>05-08-2025 16:05</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>"СовЭкон" снизил прогноз сбора пшеницы в России в 2025 году до 83,3 млн т</t>
+          <t>Расходы на кибербезопасность планируют повысить свыше 80% российских авиакомпаний</t>
         </is>
       </c>
       <c r="B22" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039263</t>
+          <t>https://www.interfax.ru/business/1039744</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>01-08-2025 16:10</t>
+          <t>05-08-2025 15:54</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>Результаты Colgate-Palmolive во II квартале превзошли прогнозы</t>
+          <t>Объем сделок M&amp;A в мире в январе-июле достиг рекорда за четыре года</t>
         </is>
       </c>
       <c r="B23" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039262</t>
+          <t>https://www.interfax.ru/business/1039742</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>01-08-2025 16:05</t>
+          <t>05-08-2025 15:34</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>В США в июле число рабочих мест выросло слабее прогноза</t>
+          <t>Segezha намерена утроить выпуск белой мешочной бумаги, в будущем рассчитывает на 20% мирового рынка</t>
         </is>
       </c>
       <c r="B24" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039261</t>
+          <t>https://www.interfax.ru/business/1039741</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>01-08-2025 15:55</t>
+          <t>05-08-2025 15:28</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Полугодовая чистая прибыль "Т Плюс" по РСБУ снизилась в 1,74 раза</t>
+          <t>США разрешили Venture Globаl допэкспорт 0,5 млрд куб. м СПГ в год с проекта Calcasieu Pass</t>
         </is>
       </c>
       <c r="B25" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039260</t>
+          <t>https://www.interfax.ru/world/1039740</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>01-08-2025 15:51</t>
+          <t>05-08-2025 15:25</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Чистый убыток "СПБ биржи" по РСБУ за I полугодие сократился в 2,3 раза</t>
+          <t>Глава ВЭБа заявил о поиске новых источников капитала для наращивания портфеля</t>
         </is>
       </c>
       <c r="B26" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039259</t>
+          <t>https://www.interfax.ru/russia/1039738</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>01-08-2025 15:49</t>
+          <t>05-08-2025 15:18</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Акционеры ТМК одобрили переход на единую акцию</t>
+          <t>Владелец KFC увеличил квартальную чистую прибыль и выручку</t>
         </is>
       </c>
       <c r="B27" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039257</t>
+          <t>https://www.interfax.ru/business/1039730</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>01-08-2025 15:46</t>
+          <t>05-08-2025 15:01</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>"Восьмерка" ОПЕК+ обсудит необходимость наращивания нефтедобычи в сентябре на 548 тыс. б/с</t>
+          <t>Чистая прибыль ХК "Новотранс" по РСБУ снизилась в I полугодии в 2,2 раза, выручка – в 1,5 раза</t>
         </is>
       </c>
       <c r="B28" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039256</t>
+          <t>https://www.interfax.ru/business/1039735</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>01-08-2025 15:39</t>
+          <t>05-08-2025 14:59</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>Экспорт российского безалкогольного пива в I полугодии вырос на 34%</t>
+          <t>Выручка Pfizer во II квартале выросла на 10%, сильнее прогнозов</t>
         </is>
       </c>
       <c r="B29" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039251</t>
+          <t>https://www.interfax.ru/business/1039729</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>01-08-2025 15:22</t>
+          <t>05-08-2025 14:43</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>"Лаборатория Касперского" нарастила долю в Ximi Pro до 90%</t>
+          <t>Mazda в I финквартале получила чистый убыток и сократила выручку на 8,8%</t>
         </is>
       </c>
       <c r="B30" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039250</t>
+          <t>https://www.interfax.ru/world/1039724</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>01-08-2025 15:13</t>
+          <t>05-08-2025 14:27</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
-          <t>Moderna во II квартале снизила чистый убыток в 1,6 раза</t>
+          <t>Литва вложила 8,5 млн евро в инфраструктуру для подготовки военнослужащих НАТО</t>
         </is>
       </c>
       <c r="B31" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039249</t>
+          <t>https://www.interfax.ru/world/1039727</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>01-08-2025 15:10</t>
+          <t>05-08-2025 14:26</t>
         </is>
       </c>
     </row>
     <row r="32">
       <c r="A32" t="inlineStr">
         <is>
-          <t>Brent подешевела до $71,04 за баррель</t>
+          <t>Caterpillar во II квартале снизил чистую прибыль на 19%, улучшил годовой прогноз</t>
         </is>
       </c>
       <c r="B32" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039246</t>
+          <t>https://www.interfax.ru/business/1039725</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>01-08-2025 15:03</t>
+          <t>05-08-2025 14:25</t>
         </is>
       </c>
     </row>
     <row r="33">
       <c r="A33" t="inlineStr">
         <is>
-          <t>Трамп призвал совет управляющих ФРС "взять управление", если Пауэлл не снизит ставку</t>
+          <t>DuPont во II квартале снизила чистую прибыль втрое</t>
         </is>
       </c>
       <c r="B33" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039237</t>
+          <t>https://www.interfax.ru/business/1039723</t>
         </is>
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>01-08-2025 14:43</t>
+          <t>05-08-2025 14:13</t>
         </is>
       </c>
     </row>
     <row r="34">
       <c r="A34" t="inlineStr">
         <is>
-          <t>В Индии надеются на продолжение переговоров с США о пошлинах</t>
+          <t>АЕБ надеется, что тренд на оживление российского авторынка будет долгосрочным</t>
         </is>
       </c>
       <c r="B34" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039232</t>
+          <t>https://www.interfax.ru/business/1039722</t>
         </is>
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>01-08-2025 14:32</t>
+          <t>05-08-2025 14:03</t>
         </is>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="inlineStr">
         <is>
-          <t>Exxon Mobil сократила чистую прибыль на 23% во II кв., лучше прогнозов</t>
+          <t>Австралия может ввести ценовые минимумы для редкоземельных металлов</t>
         </is>
       </c>
       <c r="B35" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039233</t>
+          <t>https://www.interfax.ru/business/1039721</t>
         </is>
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>01-08-2025 14:30</t>
+          <t>05-08-2025 13:54</t>
         </is>
       </c>
     </row>
     <row r="36">
       <c r="A36" t="inlineStr">
         <is>
-          <t>Nippon Steel отчиталась о чистом квартальном убытке из-за покупки US Steel</t>
+          <t>LG и Eni построят первый в Корее завод по производству биотоплива</t>
         </is>
       </c>
       <c r="B36" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039231</t>
+          <t>https://www.interfax.ru/business/1039720</t>
         </is>
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>01-08-2025 14:20</t>
+          <t>05-08-2025 13:50</t>
         </is>
       </c>
     </row>
     <row r="37">
       <c r="A37" t="inlineStr">
         <is>
-          <t>Universal Music во II квартале увеличила выручку на 1,6%</t>
+          <t>В Великобритании в июле продажи легковых машин сократились на 5%</t>
         </is>
       </c>
       <c r="B37" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039229</t>
+          <t>https://www.interfax.ru/business/1039716</t>
         </is>
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>01-08-2025 14:15</t>
+          <t>05-08-2025 13:44</t>
         </is>
       </c>
     </row>
     <row r="38">
       <c r="A38" t="inlineStr">
         <is>
-          <t>Пакистан удовлетворен торговым соглашением с США и пошлинами в 19%</t>
+          <t>"Вымпелком" создал СП для международного проекта для иностранных клиентов</t>
         </is>
       </c>
       <c r="B38" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039226</t>
+          <t>https://www.interfax.ru/business/1039713</t>
         </is>
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>01-08-2025 14:00</t>
+          <t>05-08-2025 13:16</t>
         </is>
       </c>
     </row>
     <row r="39">
       <c r="A39" t="inlineStr">
         <is>
-          <t>Chevron во II квартале сократила чистую прибыль почти вдвое</t>
+          <t>Visa собралась перенести европейскую штаб-квартиру в лондонский район Канэри-Уорф</t>
         </is>
       </c>
       <c r="B39" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039224</t>
+          <t>https://www.interfax.ru/world/1039712</t>
         </is>
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>01-08-2025 13:49</t>
+          <t>05-08-2025 13:13</t>
         </is>
       </c>
     </row>
     <row r="40">
       <c r="A40" t="inlineStr">
         <is>
-          <t>Россия и Китай договорились ускорить отмену барьеров для импорта российских пеллет</t>
+          <t>Структура АФК "Система" построит гостиничный комплекс на курорте Шерегеш</t>
         </is>
       </c>
       <c r="B40" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/russia/1039222</t>
+          <t>https://www.interfax.ru/russia/1039708</t>
         </is>
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>01-08-2025 13:47</t>
+          <t>05-08-2025 12:52</t>
         </is>
       </c>
     </row>
     <row r="41">
       <c r="A41" t="inlineStr">
         <is>
-          <t>"Яковлев" в I полугодии нарастил чистый убыток по РСБУ в 9,2 раза</t>
+          <t>"Газпром нефть" надеется получить 20 млн т дополнительной нефтедобычи</t>
         </is>
       </c>
       <c r="B41" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039223</t>
+          <t>https://www.interfax.ru/business/1039702</t>
         </is>
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>01-08-2025 13:46</t>
+          <t>05-08-2025 12:34</t>
         </is>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="inlineStr">
         <is>
-          <t>Novo Nordisk покинула топ-10 самых дорогих компаний Европы</t>
+          <t>TSMC выявила потенциальные утечки коммерческой тайны</t>
         </is>
       </c>
       <c r="B42" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039219</t>
+          <t>https://www.interfax.ru/business/1039700</t>
         </is>
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>01-08-2025 13:33</t>
+          <t>05-08-2025 12:22</t>
         </is>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="inlineStr">
         <is>
-          <t>Goldman Sachs может инвестировать в производителя мороженого Froneri</t>
+          <t>Нефтяники в июле получили почти 60 млрд руб. по демпферу</t>
         </is>
       </c>
       <c r="B43" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039212</t>
+          <t>https://www.interfax.ru/business/1039693</t>
         </is>
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>01-08-2025 13:13</t>
+          <t>05-08-2025 12:18</t>
         </is>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="inlineStr">
         <is>
-          <t>"Группа Позитив" нарастила квартальную выручку на 42% до 4,41 млрд рублей</t>
+          <t>ОТП банк в I полугодии увеличил чистую прибыль по МСФО почти вдвое</t>
         </is>
       </c>
       <c r="B44" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039208</t>
+          <t>https://www.interfax.ru/business/1039689</t>
         </is>
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>01-08-2025 13:02</t>
+          <t>05-08-2025 11:50</t>
         </is>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="inlineStr">
         <is>
-          <t>Объем торгов на СПБ бирже в июле вырос на 5% м/м, до 133,5 млрд рублей</t>
+          <t>Continental увеличил квартальную чистую прибыль в 1,7 раза</t>
         </is>
       </c>
       <c r="B45" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039202</t>
+          <t>https://www.interfax.ru/business/1039687</t>
         </is>
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>01-08-2025 12:28</t>
+          <t>05-08-2025 11:35</t>
         </is>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="inlineStr">
         <is>
-          <t>Strategy получила $14 млрд операционной прибыли во II кв. за счет роста биткойна</t>
+          <t>Квартальная прибыль DHL выросла на 9,5% при сокращении выручки</t>
         </is>
       </c>
       <c r="B46" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039181</t>
+          <t>https://www.interfax.ru/business/1039680</t>
         </is>
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>01-08-2025 10:39</t>
+          <t>05-08-2025 11:05</t>
         </is>
       </c>
     </row>
     <row r="47">
       <c r="A47" t="inlineStr">
         <is>
-          <t>Рубль утром в пятницу не демонстрирует ярко выраженной динамики на МосБирже</t>
+          <t>Hugo Boss во II квартале нарастил чистую прибыль на 27%, выручка превысила прогноз</t>
         </is>
       </c>
       <c r="B47" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039178</t>
+          <t>https://www.interfax.ru/business/1039679</t>
         </is>
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>01-08-2025 10:20</t>
+          <t>05-08-2025 11:00</t>
         </is>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="inlineStr">
         <is>
-          <t>Рынок акций РФ открылся в основную сессию ростом индексов МосБиржи и РТС на 0,7%</t>
+          <t>Diageo сократил годовую чистую прибыль на 39% при выручке лучше прогнозов</t>
         </is>
       </c>
       <c r="B48" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039176</t>
+          <t>https://www.interfax.ru/business/1039675</t>
         </is>
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>01-08-2025 10:10</t>
+          <t>05-08-2025 10:53</t>
         </is>
       </c>
     </row>
     <row r="49">
       <c r="A49" t="inlineStr">
         <is>
-          <t>Чистая прибыль "Татнефти" по РСБУ в I полугодии снизилась в 1,7 раза</t>
+          <t>Производитель полупроводников Infineon сократил квартальную чистую прибыль на 24%</t>
         </is>
       </c>
       <c r="B49" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039174</t>
+          <t>https://www.interfax.ru/business/1039670</t>
         </is>
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>01-08-2025 09:59</t>
+          <t>05-08-2025 10:32</t>
         </is>
       </c>
     </row>
     <row r="50">
       <c r="A50" t="inlineStr">
         <is>
-          <t>Озон банк начал выпускать кредитные карты</t>
+          <t>Чистая прибыль Saudi Aramco во II квартале снизилась на 22% в годовом выражении</t>
         </is>
       </c>
       <c r="B50" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039169</t>
+          <t>https://www.interfax.ru/business/1039669</t>
         </is>
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>01-08-2025 09:15</t>
+          <t>05-08-2025 10:25</t>
         </is>
       </c>
     </row>
     <row r="51">
       <c r="A51" t="inlineStr">
         <is>
-          <t>Индекс PMI обрабатывающих отраслей РФ в июле снизился до 47 пунктов</t>
+          <t>Курс рубля на "Мосбирже" не показывает ярко выраженную динамику</t>
         </is>
       </c>
       <c r="B51" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039168</t>
+          <t>https://www.interfax.ru/business/1039668</t>
         </is>
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>01-08-2025 09:09</t>
+          <t>05-08-2025 10:21</t>
         </is>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="inlineStr">
         <is>
-          <t>Amazon увеличила выручку на 13% во II квартале, лучше прогнозов</t>
+          <t>Рынок акций РФ открылся в основную сессию ростом индексов МосБиржи и РТС на 0,3%</t>
         </is>
       </c>
       <c r="B52" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039166</t>
+          <t>https://www.interfax.ru/business/1039665</t>
         </is>
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>01-08-2025 09:04</t>
+          <t>05-08-2025 10:13</t>
         </is>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="inlineStr">
         <is>
-          <t>Apple увеличила чистую прибыль в III финквартале на 9%, выручку - на 10%</t>
+          <t>BP во II квартале получила чистую прибыль</t>
         </is>
       </c>
       <c r="B53" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039165</t>
+          <t>https://www.interfax.ru/business/1039664</t>
         </is>
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>01-08-2025 08:39</t>
+          <t>05-08-2025 10:06</t>
         </is>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="inlineStr">
         <is>
-          <t>Brent подорожала до $71,84 за баррель</t>
+          <t>Выручка группы "Солар" во II квартале выросла на 44%, до 5,42 млрд рублей</t>
         </is>
       </c>
       <c r="B54" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/business/1039164</t>
+          <t>https://www.interfax.ru/business/1039663</t>
         </is>
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>01-08-2025 08:35</t>
+          <t>05-08-2025 10:02</t>
         </is>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="inlineStr">
         <is>
-          <t>Рынок акций США в четверг снизился на статданных, корпоративных отчетностях</t>
+          <t>Индекс PMI сферы услуг РФ в июле снизился до 48,6 пункта с 49,2 пункта в июне</t>
         </is>
       </c>
       <c r="B55" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/world/1039153</t>
+          <t>https://www.interfax.ru/business/1039657</t>
         </is>
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>01-08-2025 06:32</t>
+          <t>05-08-2025 09:11</t>
         </is>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="inlineStr">
         <is>
-          <t>Европейские рынки акций в основном завершили торги в минусе</t>
+          <t>Нефть продолжает дешеветь, Brent торгуется у $68,7 за баррель</t>
         </is>
       </c>
       <c r="B56" s="2" t="inlineStr">
         <is>
-          <t>https://www.interfax.ru/world/1039150</t>
+          <t>https://www.interfax.ru/business/1039654</t>
         </is>
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>01-08-2025 06:11</t>
+          <t>05-08-2025 08:34</t>
+        </is>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>"Росатом" ведет работу по выпуску облигаций в юанях и исламских облигаций, отобрал ряд компаний для выхода на IPO</t>
+        </is>
+      </c>
+      <c r="B57" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039628</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>04-08-2025 21:46</t>
+        </is>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Нидерланды, Норвегия, Португалия и ФРГ провели военно-морские учения в Арктике</t>
+        </is>
+      </c>
+      <c r="B58" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039620</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>04-08-2025 19:54</t>
+        </is>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Бензин на АЗС Москвы подорожал за июль и первые дни августа на рубль</t>
+        </is>
+      </c>
+      <c r="B59" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039618</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>04-08-2025 19:49</t>
+        </is>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Рубль практически не изменился на валютных торгах в ожидании геополитических новостей</t>
+        </is>
+      </c>
+      <c r="B60" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039619</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>04-08-2025 19:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Менеджмент "Норникеля" сохраняет среднесрочную цель снизить оборотный капитал на $1 млрд</t>
+        </is>
+      </c>
+      <c r="B61" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039613</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>04-08-2025 19:19</t>
+        </is>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>Цены на нефть замедлили снижение после заявлений Трампа</t>
+        </is>
+      </c>
+      <c r="B62" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039612</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>04-08-2025 19:13</t>
+        </is>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>Индекс Мосбиржи начал неделю с роста выше 2770 пунктов в рамках коррекции</t>
+        </is>
+      </c>
+      <c r="B63" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039611</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>04-08-2025 19:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>BP начинает добычу нефти в рамках расширения проекта Argos в Мексиканском заливе</t>
+        </is>
+      </c>
+      <c r="B64" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039610</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>04-08-2025 19:03</t>
+        </is>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>UBS заплатит $300 млн для урегулирования обязательств Credit Suisse в США</t>
+        </is>
+      </c>
+      <c r="B65" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039609</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>04-08-2025 18:53</t>
+        </is>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>Минэнерго назвало стабильной ситуацию на российском рынке нефтепродуктов</t>
+        </is>
+      </c>
+      <c r="B66" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/russia/1039608</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>04-08-2025 18:47</t>
+        </is>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>Lyft развернет роботакси в Европе в партнерстве с Baidu</t>
+        </is>
+      </c>
+      <c r="B67" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039606</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>04-08-2025 18:33</t>
+        </is>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>Швейцария не будет вводить ответные пошлины на товары из США</t>
+        </is>
+      </c>
+      <c r="B68" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039601</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>04-08-2025 18:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>Alphabet во II квартале полностью вышла из акций CrowdStrike</t>
+        </is>
+      </c>
+      <c r="B69" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039602</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>04-08-2025 18:08</t>
+        </is>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>Brent подешевела до $68,4 за баррель</t>
+        </is>
+      </c>
+      <c r="B70" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039600</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>04-08-2025 17:50</t>
+        </is>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>Биржевой товарооборот Белоруссии с Россией вырос до $634 млн</t>
+        </is>
+      </c>
+      <c r="B71" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039598</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>04-08-2025 17:20</t>
+        </is>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>Отраслевые ассоциации заявили о необходимости отдельного федерального проекта по садоводству</t>
+        </is>
+      </c>
+      <c r="B72" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/russia/1039597</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>04-08-2025 17:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>Биржевой товарооборот Белоруссии с РФ вырос до $634 млн</t>
+        </is>
+      </c>
+      <c r="B73" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039595</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>04-08-2025 17:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>BioNTech во II квартале нарастила выручку и снизила чистый убыток</t>
+        </is>
+      </c>
+      <c r="B74" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039590</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>04-08-2025 16:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>Международный суд отклонил второй иск Карапетяна о национализации в Армении ЭСА</t>
+        </is>
+      </c>
+      <c r="B75" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/world/1039587</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>04-08-2025 16:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>Таганрогский авиационный комплекс сообщил о 1,8 млрд рублей полугодового чистого убытка</t>
+        </is>
+      </c>
+      <c r="B76" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039586</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>04-08-2025 16:06</t>
+        </is>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>Садоводы Ставрополья ждут увеличения урожая яблок</t>
+        </is>
+      </c>
+      <c r="B77" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/russia/1039585</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>04-08-2025 15:59</t>
+        </is>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>Панама прекратит регистрацию 15-летних танкеров и балкеров для борьбы с "теневым флотом"</t>
+        </is>
+      </c>
+      <c r="B78" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/world/1039539</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>04-08-2025 15:27</t>
+        </is>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>Xiaomi выпустила голосовую ИИ-модель для автомобилей и бытовой техники</t>
+        </is>
+      </c>
+      <c r="B79" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039579</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>04-08-2025 15:25</t>
+        </is>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>Уран подешевел до $71,5 за фунт с июньских максимумов</t>
+        </is>
+      </c>
+      <c r="B80" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039577</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>04-08-2025 15:14</t>
+        </is>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>В октябре сменится CEO Harley-Davidson</t>
+        </is>
+      </c>
+      <c r="B81" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039575</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
+          <t>04-08-2025 15:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="82">
+      <c r="A82" t="inlineStr">
+        <is>
+          <t>Поставки Tesla с предприятия в Шанхае в июле снизились на 8,4%</t>
+        </is>
+      </c>
+      <c r="B82" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039570</t>
+        </is>
+      </c>
+      <c r="C82" t="inlineStr">
+        <is>
+          <t>04-08-2025 14:35</t>
+        </is>
+      </c>
+    </row>
+    <row r="83">
+      <c r="A83" t="inlineStr">
+        <is>
+          <t>Квартира в Петербурге попала в топ-5 самой дорогой "вторички" от "Домклика"</t>
+        </is>
+      </c>
+      <c r="B83" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039569</t>
+        </is>
+      </c>
+      <c r="C83" t="inlineStr">
+        <is>
+          <t>04-08-2025 14:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="84">
+      <c r="A84" t="inlineStr">
+        <is>
+          <t>Цены на нефть ускорили снижение, Brent у $68,6 за баррель</t>
+        </is>
+      </c>
+      <c r="B84" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039566</t>
+        </is>
+      </c>
+      <c r="C84" t="inlineStr">
+        <is>
+          <t>04-08-2025 14:16</t>
+        </is>
+      </c>
+    </row>
+    <row r="85">
+      <c r="A85" t="inlineStr">
+        <is>
+          <t>"Башкирская содовая компания" снизила дивиденды за 2024 год на 39%</t>
+        </is>
+      </c>
+      <c r="B85" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/russia/1039567</t>
+        </is>
+      </c>
+      <c r="C85" t="inlineStr">
+        <is>
+          <t>04-08-2025 14:09</t>
+        </is>
+      </c>
+    </row>
+    <row r="86">
+      <c r="A86" t="inlineStr">
+        <is>
+          <t>Shein оштрафован в Италии за недостоверные заявления об экологичности операций</t>
+        </is>
+      </c>
+      <c r="B86" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/world/1039564</t>
+        </is>
+      </c>
+      <c r="C86" t="inlineStr">
+        <is>
+          <t>04-08-2025 14:02</t>
+        </is>
+      </c>
+    </row>
+    <row r="87">
+      <c r="A87" t="inlineStr">
+        <is>
+          <t>СД "Яндекса" рекомендовал дивиденды по итогам I полугодия в 80 руб./акция</t>
+        </is>
+      </c>
+      <c r="B87" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039563</t>
+        </is>
+      </c>
+      <c r="C87" t="inlineStr">
+        <is>
+          <t>04-08-2025 13:42</t>
+        </is>
+      </c>
+    </row>
+    <row r="88">
+      <c r="A88" t="inlineStr">
+        <is>
+          <t>Выручка провайдера Cloud.ru в I полугодии выросла в 1,7 раза</t>
+        </is>
+      </c>
+      <c r="B88" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039559</t>
+        </is>
+      </c>
+      <c r="C88" t="inlineStr">
+        <is>
+          <t>04-08-2025 13:31</t>
+        </is>
+      </c>
+    </row>
+    <row r="89">
+      <c r="A89" t="inlineStr">
+        <is>
+          <t>Акции британских банков дорожают после судебной победы по делу об автокредитовании</t>
+        </is>
+      </c>
+      <c r="B89" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039557</t>
+        </is>
+      </c>
+      <c r="C89" t="inlineStr">
+        <is>
+          <t>04-08-2025 13:22</t>
+        </is>
+      </c>
+    </row>
+    <row r="90">
+      <c r="A90" t="inlineStr">
+        <is>
+          <t>Число нефтегазовых буровых в мире в июле выросло 2-й месяц подряд</t>
+        </is>
+      </c>
+      <c r="B90" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039555</t>
+        </is>
+      </c>
+      <c r="C90" t="inlineStr">
+        <is>
+          <t>04-08-2025 13:10</t>
+        </is>
+      </c>
+    </row>
+    <row r="91">
+      <c r="A91" t="inlineStr">
+        <is>
+          <t>ВР открыла крупнейшее за 25 лет для компании месторождение на шельфе Бразилии</t>
+        </is>
+      </c>
+      <c r="B91" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039550</t>
+        </is>
+      </c>
+      <c r="C91" t="inlineStr">
+        <is>
+          <t>04-08-2025 12:57</t>
+        </is>
+      </c>
+    </row>
+    <row r="92">
+      <c r="A92" t="inlineStr">
+        <is>
+          <t>Аналитики Goldman Sachs подтвердили прогноз цен на нефть, но видят риски для спроса</t>
+        </is>
+      </c>
+      <c r="B92" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039544</t>
+        </is>
+      </c>
+      <c r="C92" t="inlineStr">
+        <is>
+          <t>04-08-2025 12:28</t>
+        </is>
+      </c>
+    </row>
+    <row r="93">
+      <c r="A93" t="inlineStr">
+        <is>
+          <t>Калужский "Кристалл" в I полугодии увеличил чистую прибыль на 42%</t>
+        </is>
+      </c>
+      <c r="B93" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/russia/1039540</t>
+        </is>
+      </c>
+      <c r="C93" t="inlineStr">
+        <is>
+          <t>04-08-2025 12:18</t>
+        </is>
+      </c>
+    </row>
+    <row r="94">
+      <c r="A94" t="inlineStr">
+        <is>
+          <t>Экспортные цены на российскую пшеницу за неделю снизились на $3 до $237/т</t>
+        </is>
+      </c>
+      <c r="B94" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039525</t>
+        </is>
+      </c>
+      <c r="C94" t="inlineStr">
+        <is>
+          <t>04-08-2025 11:36</t>
+        </is>
+      </c>
+    </row>
+    <row r="95">
+      <c r="A95" t="inlineStr">
+        <is>
+          <t>Экспорт российских сыров в I полугодии увеличился в денежном измерении на 20%</t>
+        </is>
+      </c>
+      <c r="B95" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/russia/1039530</t>
+        </is>
+      </c>
+      <c r="C95" t="inlineStr">
+        <is>
+          <t>04-08-2025 11:26</t>
+        </is>
+      </c>
+    </row>
+    <row r="96">
+      <c r="A96" t="inlineStr">
+        <is>
+          <t>В Турции инфляция в июле замедлилась до 33,5%</t>
+        </is>
+      </c>
+      <c r="B96" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039528</t>
+        </is>
+      </c>
+      <c r="C96" t="inlineStr">
+        <is>
+          <t>04-08-2025 11:11</t>
+        </is>
+      </c>
+    </row>
+    <row r="97">
+      <c r="A97" t="inlineStr">
+        <is>
+          <t>Несколько руководителей ФРС посчитали рынок труда США устойчивым</t>
+        </is>
+      </c>
+      <c r="B97" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039511</t>
+        </is>
+      </c>
+      <c r="C97" t="inlineStr">
+        <is>
+          <t>04-08-2025 10:52</t>
+        </is>
+      </c>
+    </row>
+    <row r="98">
+      <c r="A98" t="inlineStr">
+        <is>
+          <t>Рубль утром в понедельник не демонстрирует ярко выраженной динамики на МосБирже</t>
+        </is>
+      </c>
+      <c r="B98" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039515</t>
+        </is>
+      </c>
+      <c r="C98" t="inlineStr">
+        <is>
+          <t>04-08-2025 10:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="99">
+      <c r="A99" t="inlineStr">
+        <is>
+          <t>"Уралмашзавод" в I полугодии увеличил чистую прибыль по РСБУ в 28 раз</t>
+        </is>
+      </c>
+      <c r="B99" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039516</t>
+        </is>
+      </c>
+      <c r="C99" t="inlineStr">
+        <is>
+          <t>04-08-2025 10:17</t>
+        </is>
+      </c>
+    </row>
+    <row r="100">
+      <c r="A100" t="inlineStr">
+        <is>
+          <t>В начале основной сессии индексы МосБиржи и РТС выросли на 0,1%</t>
+        </is>
+      </c>
+      <c r="B100" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039514</t>
+        </is>
+      </c>
+      <c r="C100" t="inlineStr">
+        <is>
+          <t>04-08-2025 10:12</t>
+        </is>
+      </c>
+    </row>
+    <row r="101">
+      <c r="A101" t="inlineStr">
+        <is>
+          <t>Адриана Куглер покинет совет управляющих ФРС досрочно</t>
+        </is>
+      </c>
+      <c r="B101" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/world/1039513</t>
+        </is>
+      </c>
+      <c r="C101" t="inlineStr">
+        <is>
+          <t>04-08-2025 10:01</t>
+        </is>
+      </c>
+    </row>
+    <row r="102">
+      <c r="A102" t="inlineStr">
+        <is>
+          <t>Berkshire Hathaway во II квартале сократила чистую прибыль в 2,5 раза</t>
+        </is>
+      </c>
+      <c r="B102" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039507</t>
+        </is>
+      </c>
+      <c r="C102" t="inlineStr">
+        <is>
+          <t>04-08-2025 08:40</t>
+        </is>
+      </c>
+    </row>
+    <row r="103">
+      <c r="A103" t="inlineStr">
+        <is>
+          <t>Цены на нефть снижаются после решения ОПЕК+ о наращивании добычи</t>
+        </is>
+      </c>
+      <c r="B103" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/business/1039506</t>
+        </is>
+      </c>
+      <c r="C103" t="inlineStr">
+        <is>
+          <t>04-08-2025 08:30</t>
+        </is>
+      </c>
+    </row>
+    <row r="104">
+      <c r="A104" t="inlineStr">
+        <is>
+          <t>Казахстан в июле сохранил экспорт нефти в Германию на уровне 160 тыс. тонн</t>
+        </is>
+      </c>
+      <c r="B104" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/world/1039501</t>
+        </is>
+      </c>
+      <c r="C104" t="inlineStr">
+        <is>
+          <t>04-08-2025 07:44</t>
+        </is>
+      </c>
+    </row>
+    <row r="105">
+      <c r="A105" t="inlineStr">
+        <is>
+          <t>Падение S&amp;P 500 и Nasdaq в пятницу было максимальным с апреля</t>
+        </is>
+      </c>
+      <c r="B105" s="2" t="inlineStr">
+        <is>
+          <t>https://www.interfax.ru/world/1039494</t>
+        </is>
+      </c>
+      <c r="C105" t="inlineStr">
+        <is>
+          <t>04-08-2025 06:32</t>
         </is>
       </c>
     </row>
@@ -1461,6 +2294,55 @@
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B54" tooltip="Перейти по ссылке" r:id="rId53"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B55" tooltip="Перейти по ссылке" r:id="rId54"/>
     <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B56" tooltip="Перейти по ссылке" r:id="rId55"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B57" tooltip="Перейти по ссылке" r:id="rId56"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B58" tooltip="Перейти по ссылке" r:id="rId57"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B59" tooltip="Перейти по ссылке" r:id="rId58"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B60" tooltip="Перейти по ссылке" r:id="rId59"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B61" tooltip="Перейти по ссылке" r:id="rId60"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B62" tooltip="Перейти по ссылке" r:id="rId61"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B63" tooltip="Перейти по ссылке" r:id="rId62"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B64" tooltip="Перейти по ссылке" r:id="rId63"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B65" tooltip="Перейти по ссылке" r:id="rId64"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B66" tooltip="Перейти по ссылке" r:id="rId65"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B67" tooltip="Перейти по ссылке" r:id="rId66"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B68" tooltip="Перейти по ссылке" r:id="rId67"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B69" tooltip="Перейти по ссылке" r:id="rId68"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B70" tooltip="Перейти по ссылке" r:id="rId69"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B71" tooltip="Перейти по ссылке" r:id="rId70"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B72" tooltip="Перейти по ссылке" r:id="rId71"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B73" tooltip="Перейти по ссылке" r:id="rId72"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B74" tooltip="Перейти по ссылке" r:id="rId73"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B75" tooltip="Перейти по ссылке" r:id="rId74"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B76" tooltip="Перейти по ссылке" r:id="rId75"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B77" tooltip="Перейти по ссылке" r:id="rId76"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B78" tooltip="Перейти по ссылке" r:id="rId77"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B79" tooltip="Перейти по ссылке" r:id="rId78"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B80" tooltip="Перейти по ссылке" r:id="rId79"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B81" tooltip="Перейти по ссылке" r:id="rId80"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B82" tooltip="Перейти по ссылке" r:id="rId81"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B83" tooltip="Перейти по ссылке" r:id="rId82"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B84" tooltip="Перейти по ссылке" r:id="rId83"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B85" tooltip="Перейти по ссылке" r:id="rId84"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B86" tooltip="Перейти по ссылке" r:id="rId85"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B87" tooltip="Перейти по ссылке" r:id="rId86"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B88" tooltip="Перейти по ссылке" r:id="rId87"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B89" tooltip="Перейти по ссылке" r:id="rId88"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B90" tooltip="Перейти по ссылке" r:id="rId89"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B91" tooltip="Перейти по ссылке" r:id="rId90"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B92" tooltip="Перейти по ссылке" r:id="rId91"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B93" tooltip="Перейти по ссылке" r:id="rId92"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B94" tooltip="Перейти по ссылке" r:id="rId93"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B95" tooltip="Перейти по ссылке" r:id="rId94"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B96" tooltip="Перейти по ссылке" r:id="rId95"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B97" tooltip="Перейти по ссылке" r:id="rId96"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B98" tooltip="Перейти по ссылке" r:id="rId97"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B99" tooltip="Перейти по ссылке" r:id="rId98"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B100" tooltip="Перейти по ссылке" r:id="rId99"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B101" tooltip="Перейти по ссылке" r:id="rId100"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B102" tooltip="Перейти по ссылке" r:id="rId101"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B103" tooltip="Перейти по ссылке" r:id="rId102"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B104" tooltip="Перейти по ссылке" r:id="rId103"/>
+    <hyperlink xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ref="B105" tooltip="Перейти по ссылке" r:id="rId104"/>
   </hyperlinks>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>